<commit_message>
Added stunt runs w/ some destinations
Also adjusted how destinations are calculated
</commit_message>
<xml_diff>
--- a/map_data.xlsx
+++ b/map_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-3160" windowWidth="19200" windowHeight="19700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
   <si>
     <t>X Coordinate</t>
   </si>
@@ -437,6 +437,93 @@
   </si>
   <si>
     <t>Hamilton &amp; 5th</t>
+  </si>
+  <si>
+    <t>About Town</t>
+  </si>
+  <si>
+    <t>Stunt Run</t>
+  </si>
+  <si>
+    <t>Chubb &amp; West Lake</t>
+  </si>
+  <si>
+    <t>Base Jumper</t>
+  </si>
+  <si>
+    <t>South Rouse &amp; Ross</t>
+  </si>
+  <si>
+    <t>Bravo, Encore!</t>
+  </si>
+  <si>
+    <t>3rd &amp; Lambert</t>
+  </si>
+  <si>
+    <t>Cliffhanger</t>
+  </si>
+  <si>
+    <t>Chubb &amp; Hans</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>1st &amp; Root</t>
+  </si>
+  <si>
+    <t>Express Yourself</t>
+  </si>
+  <si>
+    <t>South Mountain &amp; South Bay Expressway</t>
+  </si>
+  <si>
+    <t>Falling Down</t>
+  </si>
+  <si>
+    <t>North Mountain &amp; Uphill</t>
+  </si>
+  <si>
+    <t>Hang 10</t>
+  </si>
+  <si>
+    <t>Lambert Parkway &amp; 9th</t>
+  </si>
+  <si>
+    <t>Lighthouse Party</t>
+  </si>
+  <si>
+    <t>Patterson &amp; 9th</t>
+  </si>
+  <si>
+    <t>Near the Edge</t>
+  </si>
+  <si>
+    <t>Nelson &amp; Read</t>
+  </si>
+  <si>
+    <t>Offroad Parking</t>
+  </si>
+  <si>
+    <t>Lambert &amp; Hall</t>
+  </si>
+  <si>
+    <t>Over Construction</t>
+  </si>
+  <si>
+    <t>Harber &amp; Warren</t>
+  </si>
+  <si>
+    <t>Rack 'Em Up</t>
+  </si>
+  <si>
+    <t>East Lake &amp; Rack</t>
+  </si>
+  <si>
+    <t>Unconventional</t>
+  </si>
+  <si>
+    <t>Andersen &amp; Angus</t>
   </si>
 </sst>
 </file>
@@ -792,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1925,6 +2012,276 @@
       </c>
       <c r="F56" s="4" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" s="4">
+        <v>314</v>
+      </c>
+      <c r="C57" s="4">
+        <v>469</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" s="4">
+        <v>802</v>
+      </c>
+      <c r="C58" s="4">
+        <v>464</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B59" s="4">
+        <v>1071</v>
+      </c>
+      <c r="C59" s="4">
+        <v>619</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="4">
+        <v>373</v>
+      </c>
+      <c r="C60" s="4">
+        <v>867</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B61" s="4">
+        <v>1377</v>
+      </c>
+      <c r="C61" s="4">
+        <v>803</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62" s="4">
+        <v>571</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1077</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B63" s="4">
+        <v>120</v>
+      </c>
+      <c r="C63" s="4">
+        <v>467</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B64" s="4">
+        <v>1091</v>
+      </c>
+      <c r="C64" s="4">
+        <v>400</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B65" s="4">
+        <v>1434</v>
+      </c>
+      <c r="C65" s="4">
+        <v>447</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B66" s="4">
+        <v>370</v>
+      </c>
+      <c r="C66" s="4">
+        <v>210</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B67" s="4">
+        <v>900</v>
+      </c>
+      <c r="C67" s="4">
+        <v>913</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B68" s="4">
+        <v>1109</v>
+      </c>
+      <c r="C68" s="4">
+        <v>867</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B69" s="4">
+        <v>636</v>
+      </c>
+      <c r="C69" s="4">
+        <v>586</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" s="4">
+        <v>1560</v>
+      </c>
+      <c r="C70" s="4">
+        <v>652</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1974,6 +2331,11 @@
     <hyperlink ref="A52" r:id="rId43" tooltip="Safe Harbor"/>
     <hyperlink ref="A53" r:id="rId44" tooltip="Seeing Stars"/>
     <hyperlink ref="A56" r:id="rId45" tooltip="Strike Out"/>
+    <hyperlink ref="A60" r:id="rId46" tooltip="Cliffhanger (Burnout Paradise)"/>
+    <hyperlink ref="A62" r:id="rId47" tooltip="Express Yourself"/>
+    <hyperlink ref="A63" r:id="rId48" tooltip="Falling Down (Burnout Paradise)"/>
+    <hyperlink ref="A64" r:id="rId49" tooltip="Hang 10"/>
+    <hyperlink ref="A68" r:id="rId50" tooltip="Over Construction"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added search box for events w/ autocomplete
</commit_message>
<xml_diff>
--- a/map_data.xlsx
+++ b/map_data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="165">
   <si>
     <t>X Coordinate</t>
   </si>
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2447,10 +2447,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2459,7 +2459,7 @@
     <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -2469,8 +2469,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -2480,8 +2483,11 @@
       <c r="C2">
         <v>278</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -2491,8 +2497,11 @@
       <c r="C3">
         <v>369</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2502,8 +2511,11 @@
       <c r="C4">
         <v>654</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -2513,8 +2525,11 @@
       <c r="C5">
         <v>816</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2524,8 +2539,11 @@
       <c r="C6">
         <v>1050</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -2535,8 +2553,11 @@
       <c r="C7">
         <v>1122</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -2546,8 +2567,11 @@
       <c r="C8">
         <v>468</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2556,6 +2580,9 @@
       </c>
       <c r="C9">
         <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>